<commit_message>
Actually good converged atmosphere
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK_VENUS.xlsx
+++ b/REACTION_NETWORK_VENUS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
@@ -1221,7 +1221,7 @@
     <t xml:space="preserve">Ions</t>
   </si>
   <si>
-    <t xml:space="preserve">New</t>
+    <t xml:space="preserve">Conv</t>
   </si>
   <si>
     <t xml:space="preserve">CO2plpl</t>
@@ -1374,10 +1374,10 @@
   <dimension ref="A1:Y280"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E36 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -17330,10 +17330,10 @@
   <dimension ref="A1:AF681"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="1" sqref="E2:E36 G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -61741,11 +61741,11 @@
   </sheetPr>
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E2:E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -61815,7 +61815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -61841,7 +61841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -61867,7 +61867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
@@ -61945,7 +61945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
@@ -61971,7 +61971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -62006,7 +62006,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -62041,7 +62041,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
@@ -62076,7 +62076,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -62111,7 +62111,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
@@ -62146,7 +62146,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
@@ -62172,7 +62172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>75</v>
       </c>
@@ -62198,7 +62198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -62233,7 +62233,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -62268,7 +62268,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
@@ -62303,7 +62303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -62338,7 +62338,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
@@ -62373,7 +62373,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>90</v>
       </c>
@@ -62408,7 +62408,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>90</v>
       </c>
@@ -62434,7 +62434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>90</v>
       </c>
@@ -62469,7 +62469,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>90</v>
       </c>
@@ -62495,7 +62495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
@@ -62547,7 +62547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
@@ -62599,7 +62599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
@@ -62625,7 +62625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
@@ -62651,7 +62651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>85</v>
       </c>
@@ -62677,7 +62677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>85</v>
       </c>
@@ -62703,7 +62703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
@@ -62729,7 +62729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -62764,7 +62764,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
@@ -62799,7 +62799,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -62834,7 +62834,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>52</v>
       </c>
@@ -62887,11 +62887,11 @@
   </sheetPr>
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -62961,7 +62961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -62987,7 +62987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -63013,7 +63013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -63039,7 +63039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
@@ -63065,7 +63065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -63091,7 +63091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>63</v>
       </c>
@@ -63117,7 +63117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
@@ -63143,7 +63143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
@@ -63169,7 +63169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -63195,7 +63195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>71</v>
       </c>
@@ -63224,7 +63224,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -63253,7 +63253,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -63279,7 +63279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -63317,7 +63317,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -63358,7 +63358,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -63399,7 +63399,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>79</v>
       </c>
@@ -63425,7 +63425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
@@ -63454,7 +63454,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -63492,7 +63492,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>79</v>
       </c>
@@ -63530,7 +63530,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
@@ -63559,7 +63559,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -63585,7 +63585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -63611,7 +63611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -63643,7 +63643,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -63675,7 +63675,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -63716,7 +63716,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>76</v>
       </c>
@@ -63757,7 +63757,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -63795,7 +63795,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -63821,7 +63821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -63847,7 +63847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>131</v>
       </c>
@@ -63873,7 +63873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -63899,7 +63899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -63925,7 +63925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -63951,7 +63951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>
@@ -63977,7 +63977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
@@ -64022,10 +64022,10 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E36 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -65747,10 +65747,10 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:E36 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Final changes before resubmission--- updated HDO/H2O, HCO+ + e- branching ratio, resized plots, fixed bug in generating LaTeX output for reaction tables
</commit_message>
<xml_diff>
--- a/REACTION_NETWORK_VENUS.xlsx
+++ b/REACTION_NETWORK_VENUS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" state="visible" r:id="rId2"/>
@@ -1367,11 +1367,11 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="S647 A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -17164,11 +17164,11 @@
   </sheetPr>
   <dimension ref="A1:AF681"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A616" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A585" activeCellId="0" sqref="A585"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R632" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S647" activeCellId="0" sqref="S647"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -59039,7 +59039,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="645" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="1" t="s">
         <v>50</v>
       </c>
@@ -59065,7 +59065,7 @@
         <v>0.01</v>
       </c>
       <c r="S645" s="1" t="n">
-        <v>1.15E-007</v>
+        <v>1.15E-005</v>
       </c>
       <c r="T645" s="1" t="n">
         <v>-0.64</v>
@@ -59101,7 +59101,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="646" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="1" t="s">
         <v>50</v>
       </c>
@@ -59139,7 +59139,7 @@
         <v>0.92</v>
       </c>
       <c r="S646" s="1" t="n">
-        <v>1.06E-005</v>
+        <v>1.15E-005</v>
       </c>
       <c r="T646" s="1" t="n">
         <v>-0.64</v>
@@ -59175,7 +59175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="647" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="1" t="s">
         <v>50</v>
       </c>
@@ -59201,7 +59201,7 @@
         <v>0.07</v>
       </c>
       <c r="S647" s="1" t="n">
-        <v>8.08E-007</v>
+        <v>1.15E-005</v>
       </c>
       <c r="T647" s="1" t="n">
         <v>-0.64</v>
@@ -61583,10 +61583,10 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S647 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -62729,10 +62729,10 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S647 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -63863,10 +63863,10 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S647 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -65588,10 +65588,10 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S647 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>